<commit_message>
adcionada descrição da entidade favoritos
</commit_message>
<xml_diff>
--- a/documentacao/banco-documentacao/dicionario_de_dados.xlsx
+++ b/documentacao/banco-documentacao/dicionario_de_dados.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\easy-park\DOCUMENTAÇAO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/pedro_souza_bandtec_com_br/Documents/1git/easy-park/DOCUMENTAÇAO/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_D072117DCDE8229418665FF8AF1F5A7D84E2959B" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0ED7B486-D072-41FE-B941-D5C4A7EB5222}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="85">
   <si>
     <t xml:space="preserve">Entidade: Usuario </t>
   </si>
@@ -171,6 +172,69 @@
   </si>
   <si>
     <t>Identificador da entidade usuarioPJ</t>
+  </si>
+  <si>
+    <t>fkEstac</t>
+  </si>
+  <si>
+    <t>fkUsuarPF</t>
+  </si>
+  <si>
+    <t>Entidade: Favorito</t>
+  </si>
+  <si>
+    <t>Entidade:Registro</t>
+  </si>
+  <si>
+    <t>idRegistro</t>
+  </si>
+  <si>
+    <t>data_hora</t>
+  </si>
+  <si>
+    <t>situacao_vaga</t>
+  </si>
+  <si>
+    <t>fkVagas</t>
+  </si>
+  <si>
+    <t>idVagas</t>
+  </si>
+  <si>
+    <t>sensor</t>
+  </si>
+  <si>
+    <t>Entidade: Vagas</t>
+  </si>
+  <si>
+    <t>id_vaga</t>
+  </si>
+  <si>
+    <t>fk_estacionamento</t>
+  </si>
+  <si>
+    <t>fk_estac</t>
+  </si>
+  <si>
+    <t>fk_user</t>
+  </si>
+  <si>
+    <t>id_registro</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>situacao</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>0 ou 1</t>
+  </si>
+  <si>
+    <t>fk_vaga</t>
   </si>
   <si>
     <r>
@@ -224,7 +288,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Carga inicial de 100 ocorrências e o volume semanal de mais 100 ocorrências.</t>
+      <t>Carga inicial de 70 ocorrências e o volume semanal de mais 100 ocorrências.</t>
     </r>
     <r>
       <rPr>
@@ -279,7 +343,189 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Entidade para registro de estacionamentos.
+      <t xml:space="preserve">Entidade fraca da tabela usuário responsavél por armazenar os das pessoas fisicas que usam o sistema  do sistema EasyPark.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nome da Tabela:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tb_PJ.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Carga inicial de 30% ocorrências e o volume semanal de mais 40% ocorrências dos registros da tabela usuário.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Tempo de retenção: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Somente quando o usuário de solicitar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Rotina de limpeza: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Somente quando necessário</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Descrição: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Entidade fraca da tabela usuário responsavél por armazenar os das pessoas fisicas que usam o sistema  do sistema EasyPark.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nome da Tabela:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tb_PF.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Carga inicial de 70% ocorrências e o volume semanal de mais 60% ocorrências dos registros da tabela usuário.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Tempo de retenção: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Somente quando o usuário de solicitar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Rotina de limpeza: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Somente quando necessário</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Descrição: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Entidade responsavél por armazenar os dados do local dos Estacionamentos cadastrados.
 </t>
     </r>
     <r>
@@ -315,7 +561,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Carga inicial de 20% ocorrências e o volume semanal de mais 20% ocorrências dos registros da tabela usuário.</t>
+      <t xml:space="preserve">Carga inicial de 30 ocorrências e o volume semanal de mais 50 ocorrências.
+</t>
     </r>
     <r>
       <rPr>
@@ -333,7 +580,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Somente quando o usuário gestor solicitar</t>
+      <t xml:space="preserve">Somente quando o usuário do tipo pessoa juridica solicitar.
+</t>
     </r>
     <r>
       <rPr>
@@ -355,15 +603,6 @@
     </r>
   </si>
   <si>
-    <t>fkEstac</t>
-  </si>
-  <si>
-    <t>fkUsuarPF</t>
-  </si>
-  <si>
-    <t>Entidade: Favorito</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -379,7 +618,213 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve"> Entidade responsavél por armazenar os dados das vagas de um determinado estacionamentos.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nome da Tabela:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> vagas
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Carga inicial de  1600 ocorrências e o volume mensal de mais 25000 ocorrências.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">
+Tempo de retenção: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Somente quando o usuário de solicitar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Rotina de limpeza: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Somente quando necessário</t>
+    </r>
+  </si>
+  <si>
+    <t>O identificador da vagas é utilizado para verificar uma ocorrência.</t>
+  </si>
+  <si>
+    <t>O identificador do registro é utilizado para verificar uma ocorrência.</t>
+  </si>
+  <si>
+    <t>Numero do sensor correspondente a vaga</t>
+  </si>
+  <si>
+    <t>Data e hora   do registro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Registro para  vaga ocupada ou livre,sendo 1 correspondendo a vaga ocupada e 0 para vaga livre  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relacionamento com tabela estacionamento </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relacionamento com tabela usuário </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relacionamento com tabela vaga </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Descrição: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Entidade responsavél por armazenar os dados os registros da tabela vagas.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nome da Tabela:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> registro
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Carga inicial de 5000 ocorrências e o volume semanal de mais 10000 ocorrências dos registros da tabela usuário.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Tempo de retenção: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Permanente</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Rotina de limpeza: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Não se aplica</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Descrição:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Entidade relacional das tabelas pt e estacionamento. Onde ficá guardado os estacionamento favoritos pelos usuarios de pessoas físicos
 </t>
     </r>
     <r>
@@ -415,7 +860,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Carga inicial de 30% ocorrências e o volume semanal de mais 30% ocorrências dos registros da tabela usuário.</t>
+      <t>Carga inicial de 10 ocorrências e o volume mensal de mais 30 ocorrências.</t>
     </r>
     <r>
       <rPr>
@@ -453,430 +898,12 @@
       </rPr>
       <t>Somente quando necessário</t>
     </r>
-  </si>
-  <si>
-    <t>Entidade:Registro</t>
-  </si>
-  <si>
-    <t>idRegistro</t>
-  </si>
-  <si>
-    <t>data_hora</t>
-  </si>
-  <si>
-    <t>situacao_vaga</t>
-  </si>
-  <si>
-    <t>fkVagas</t>
-  </si>
-  <si>
-    <t>idVagas</t>
-  </si>
-  <si>
-    <t>sensor</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Descrição:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Nome da Tabela:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> registro
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Volume esperado: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Carga inicial de 30% ocorrências e o volume semanal de mais 30% ocorrências dos registros da tabela usuário.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Tempo de retenção: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Somente quando o usuário de solicitar</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Rotina de limpeza: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Somente quando necessário</t>
-    </r>
-  </si>
-  <si>
-    <t>Entidade: Vagas</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Descrição:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Nome da Tabela:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> vagas
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Volume esperado: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Carga inicial de 30% ocorrências e o volume semanal de mais 30% ocorrências dos registros da tabela usuário.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Tempo de retenção: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Somente quando o usuário de solicitar</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Rotina de limpeza: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Somente quando necessário</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Descrição: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Entidade fraca da tabela usuário responsavél por armazenar os das pessoas fisicas que usam o sistema  do sistema EasyPark.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Nome da Tabela:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tb_PF.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Volume esperado: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Carga inicial de 70% ocorrências e o volume semanal de mais 70% ocorrências dos registros da tabela usuário.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Tempo de retenção: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Somente quando o usuário de solicitar</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Rotina de limpeza: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Somente quando necessário</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Descrição: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Entidade fraca da tabela usuário responsavél por armazenar os das pessoas fisicas que usam o sistema  do sistema EasyPark.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Nome da Tabela:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tb_PJ.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Volume esperado: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Carga inicial de 30% ocorrências e o volume semanal de mais 30% ocorrências dos registros da tabela usuário.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Tempo de retenção: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Somente quando o usuário de solicitar</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Rotina de limpeza: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Somente quando necessário</t>
-    </r>
-  </si>
-  <si>
-    <t>id_vaga</t>
-  </si>
-  <si>
-    <t>fk_estacionamento</t>
-  </si>
-  <si>
-    <t>fk_estac</t>
-  </si>
-  <si>
-    <t>fk_user</t>
-  </si>
-  <si>
-    <t>id_registro</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>situacao</t>
-  </si>
-  <si>
-    <t>bit</t>
-  </si>
-  <si>
-    <t>0 ou 1</t>
-  </si>
-  <si>
-    <t>fk_vaga</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -936,7 +963,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1177,31 +1204,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1254,21 +1261,24 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1277,15 +1287,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1591,21 +1592,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
     <col min="5" max="6" width="27.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="41.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="49.7109375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1616,16 +1617,16 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32" t="s">
-        <v>49</v>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1647,7 +1648,7 @@
       <c r="G3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="33"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1668,7 +1669,7 @@
       <c r="G4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="33"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -1689,7 +1690,7 @@
       <c r="G5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="33"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
@@ -1710,7 +1711,7 @@
       <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="33"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
@@ -1731,23 +1732,23 @@
       <c r="G7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="34"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="21" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1772,10 +1773,10 @@
       <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1787,7 +1788,9 @@
       <c r="F11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="18"/>
+      <c r="G11" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1809,23 +1812,23 @@
       <c r="G12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="26"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
       <c r="H14" s="21" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1850,10 +1853,10 @@
       <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8" s="16" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="18" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1865,7 +1868,9 @@
       <c r="F16" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="18"/>
+      <c r="G16" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="H16" s="22"/>
     </row>
     <row r="17" spans="2:8" s="2" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1887,23 +1892,23 @@
       <c r="G17" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="26"/>
+      <c r="H17" s="23"/>
     </row>
     <row r="18" spans="2:8" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="27" t="s">
-        <v>50</v>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="21" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1925,10 +1930,10 @@
       <c r="G20" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="28"/>
+      <c r="H20" s="22"/>
     </row>
     <row r="21" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1946,10 +1951,10 @@
       <c r="G21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="28"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="2:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1967,10 +1972,10 @@
       <c r="G22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="28"/>
+      <c r="H22" s="22"/>
     </row>
     <row r="23" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -1988,10 +1993,10 @@
       <c r="G23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H23" s="28"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -2009,41 +2014,41 @@
       <c r="G24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="28"/>
-    </row>
-    <row r="25" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="2:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="28"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="25"/>
+      <c r="B27" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
       <c r="H27" s="21" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2068,11 +2073,11 @@
       <c r="H28" s="22"/>
     </row>
     <row r="29" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
-        <v>51</v>
+      <c r="B29" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>43</v>
@@ -2083,40 +2088,44 @@
       <c r="F29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="H29" s="22"/>
     </row>
     <row r="30" spans="2:8" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="B30" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="26"/>
+      <c r="G30" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H30" s="23"/>
     </row>
     <row r="31" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="25"/>
+      <c r="B32" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="26"/>
       <c r="H32" s="21" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2141,33 +2150,35 @@
       <c r="H33" s="22"/>
     </row>
     <row r="34" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>71</v>
+      <c r="B34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="E34" s="6">
+        <v>5</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="18"/>
+      <c r="G34" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="H34" s="22"/>
     </row>
     <row r="35" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="20" t="s">
-        <v>57</v>
+      <c r="B35" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>8</v>
@@ -2175,138 +2186,150 @@
       <c r="F35" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="6"/>
+      <c r="G35" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="H35" s="22"/>
     </row>
-    <row r="36" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F36" s="6" t="s">
+    <row r="36" spans="2:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" s="23"/>
+    </row>
+    <row r="37" spans="2:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="22"/>
-    </row>
-    <row r="37" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="22"/>
-    </row>
-    <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" s="22"/>
-    </row>
-    <row r="41" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="G41" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="6">
-        <v>5</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="6"/>
-      <c r="H41" s="22"/>
-    </row>
-    <row r="42" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="E42" s="6" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="6"/>
+      <c r="G42" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="H42" s="22"/>
     </row>
-    <row r="43" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="6" t="s">
+    <row r="43" spans="2:8" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
+      <c r="G43" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H43" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2316,16 +2339,16 @@
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:H7"/>
     <mergeCell ref="B9:G9"/>
-    <mergeCell ref="H32:H37"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="H39:H43"/>
+    <mergeCell ref="H38:H43"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="H32:H36"/>
     <mergeCell ref="H27:H30"/>
     <mergeCell ref="H19:H25"/>
     <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B38:G38"/>
     <mergeCell ref="B19:G19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>